<commit_message>
Debugged mycart page and working on excel functionality
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -12,30 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
-    <t>Head First Java</t>
-  </si>
-  <si>
-    <t>Kathy Serria</t>
-  </si>
-  <si>
-    <t>Effective Java</t>
-  </si>
-  <si>
-    <t>Joshua Bloch</t>
-  </si>
-  <si>
-    <t>Clean Code</t>
-  </si>
-  <si>
-    <t>Robert martin</t>
-  </si>
-  <si>
-    <t>Thinking in Java</t>
-  </si>
-  <si>
-    <t>Bruce Eckel</t>
+    <t>Downspout</t>
   </si>
 </sst>
 </file>
@@ -80,7 +59,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:D5"/>
+  <dimension ref="B2:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -90,44 +69,16 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" t="s">
-        <v>1</v>
-      </c>
-      <c r="D2" t="n">
-        <v>79.0</v>
+      <c r="C2" t="n">
+        <v>5.0</v>
       </c>
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
-      <c r="C3" t="s">
-        <v>3</v>
-      </c>
-      <c r="D3" t="n">
-        <v>36.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="s">
-        <v>4</v>
-      </c>
-      <c r="C4" t="s">
-        <v>5</v>
-      </c>
-      <c r="D4" t="n">
-        <v>42.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="B5" t="s">
-        <v>6</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-      <c r="D5" t="n">
-        <v>35.0</v>
+      <c r="C3" t="n">
+        <v>10.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Submit and email excel feature is fully functional
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -12,9 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
   <si>
-    <t>Downspout</t>
+    <t>DS2310BLK-LF</t>
+  </si>
+  <si>
+    <t>DS2310WMUS-LF</t>
   </si>
 </sst>
 </file>
@@ -59,7 +62,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:C3"/>
+  <dimension ref="B2:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -75,10 +78,18 @@
     </row>
     <row r="3">
       <c r="B3" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="C3" t="n">
         <v>10.0</v>
+      </c>
+    </row>
+    <row r="4">
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" t="n">
+        <v>4.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added character requirements for signup forms, fixed minor css flaws
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -12,12 +12,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>DS2310BLK-LF</t>
+    <t>DS2310LGWHT-LF</t>
   </si>
   <si>
-    <t>DS2310WMUS-LF</t>
+    <t>DS3410LGWHT-LF</t>
   </si>
 </sst>
 </file>
@@ -62,7 +62,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:C4"/>
+  <dimension ref="B2:C3"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -73,7 +73,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>5.0</v>
+        <v>3.0</v>
       </c>
     </row>
     <row r="3">
@@ -81,15 +81,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" t="n">
-        <v>4.0</v>
+        <v>1.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added logic to consolidate lineItem if user adds the same item to the cart more than once
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -14,10 +14,10 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>DS2310LGWHT-LF</t>
+    <t>DS2310BLK-LF</t>
   </si>
   <si>
-    <t>DS3410LGWHT-LF</t>
+    <t>DS2310WMUS-LF</t>
   </si>
 </sst>
 </file>
@@ -73,7 +73,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>3.0</v>
+        <v>5.0</v>
       </c>
     </row>
     <row r="3">
@@ -81,7 +81,7 @@
         <v>1</v>
       </c>
       <c r="C3" t="n">
-        <v>1.0</v>
+        <v>243.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added admin accessto add/edit/delete products and would reflect on everyone's product/cart page
</commit_message>
<xml_diff>
--- a/order.xlsx
+++ b/order.xlsx
@@ -12,12 +12,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
   <si>
     <t>DS2310BLK-LF</t>
-  </si>
-  <si>
-    <t>DS2310WMUS-LF</t>
   </si>
 </sst>
 </file>
@@ -62,7 +59,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:C3"/>
+  <dimension ref="B2:C2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -73,15 +70,7 @@
         <v>0</v>
       </c>
       <c r="C2" t="n">
-        <v>5.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="B3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C3" t="n">
-        <v>243.0</v>
+        <v>32.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>